<commit_message>
Update SEED LAB HMM Submission Sheet for 202405 with new data
</commit_message>
<xml_diff>
--- a/metadata/SEED LAB HMM Submission Sheet 202405.xlsx
+++ b/metadata/SEED LAB HMM Submission Sheet 202405.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://luriechildrens-my.sharepoint.com/personal/fimieye_luriechildrens_org/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pseed\Documents\GitHub\abbott-carbohydrate-obesity-project2\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B292FD60-33D6-4059-B0E6-12BC32F64250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DF9B77D-05ED-43FD-B49C-A393703B9B8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18080" tabRatio="211" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="211" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5657" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5653" uniqueCount="460">
   <si>
     <t>MMF logo</t>
   </si>
@@ -218,16 +218,10 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>HT</t>
-  </si>
-  <si>
     <t>58a r1 48h</t>
   </si>
   <si>
     <t>58a r2 0h</t>
-  </si>
-  <si>
-    <t>LD</t>
   </si>
   <si>
     <t>58a r2 48h</t>
@@ -2437,7 +2431,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -2481,7 +2475,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -2505,11 +2499,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:OG689"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="88" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="L2" zoomScale="88" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="U17" sqref="U17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.95"/>
+  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="39.85546875" style="3" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
@@ -5754,7 +5748,7 @@
       <c r="OF10" s="61"/>
       <c r="OG10" s="61"/>
     </row>
-    <row r="11" spans="1:397" s="9" customFormat="1" ht="27.95" hidden="1">
+    <row r="11" spans="1:397" s="9" customFormat="1" ht="38.25" hidden="1">
       <c r="A11" s="19" t="s">
         <v>48</v>
       </c>
@@ -6975,9 +6969,7 @@
         <v>500</v>
       </c>
       <c r="S14" s="37"/>
-      <c r="T14" s="37" t="s">
-        <v>58</v>
-      </c>
+      <c r="T14" s="37"/>
       <c r="U14" s="55"/>
       <c r="V14" s="56"/>
       <c r="W14" s="56"/>
@@ -7358,7 +7350,7 @@
     </row>
     <row r="15" spans="1:397" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A15" s="64" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B15" s="65" t="s">
         <v>52</v>
@@ -7408,9 +7400,7 @@
         <v>500</v>
       </c>
       <c r="S15" s="37"/>
-      <c r="T15" s="37" t="s">
-        <v>58</v>
-      </c>
+      <c r="T15" s="37"/>
       <c r="U15" s="55"/>
       <c r="V15" s="56"/>
       <c r="W15" s="56"/>
@@ -7437,7 +7427,7 @@
     </row>
     <row r="16" spans="1:397" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A16" s="64" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B16" s="65" t="s">
         <v>52</v>
@@ -7487,9 +7477,7 @@
         <v>500</v>
       </c>
       <c r="S16" s="37"/>
-      <c r="T16" s="37" t="s">
-        <v>61</v>
-      </c>
+      <c r="T16" s="37"/>
       <c r="U16" s="55"/>
       <c r="V16" s="56"/>
       <c r="W16" s="56"/>
@@ -7516,7 +7504,7 @@
     </row>
     <row r="17" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A17" s="64" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B17" s="65" t="s">
         <v>52</v>
@@ -7566,9 +7554,7 @@
         <v>500</v>
       </c>
       <c r="S17" s="37"/>
-      <c r="T17" s="37" t="s">
-        <v>61</v>
-      </c>
+      <c r="T17" s="37"/>
       <c r="U17" s="55"/>
       <c r="V17" s="56"/>
       <c r="W17" s="56"/>
@@ -7595,7 +7581,7 @@
     </row>
     <row r="18" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A18" s="64" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B18" s="65" t="s">
         <v>52</v>
@@ -7672,7 +7658,7 @@
     </row>
     <row r="19" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A19" s="64" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B19" s="65" t="s">
         <v>52</v>
@@ -7749,7 +7735,7 @@
     </row>
     <row r="20" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A20" s="64" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B20" s="65" t="s">
         <v>52</v>
@@ -7826,7 +7812,7 @@
     </row>
     <row r="21" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A21" s="64" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B21" s="65" t="s">
         <v>52</v>
@@ -7903,7 +7889,7 @@
     </row>
     <row r="22" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A22" s="64" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B22" s="65" t="s">
         <v>52</v>
@@ -7980,7 +7966,7 @@
     </row>
     <row r="23" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A23" s="64" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B23" s="65" t="s">
         <v>52</v>
@@ -8057,7 +8043,7 @@
     </row>
     <row r="24" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A24" s="64" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B24" s="65" t="s">
         <v>52</v>
@@ -8134,7 +8120,7 @@
     </row>
     <row r="25" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A25" s="64" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B25" s="65" t="s">
         <v>52</v>
@@ -8211,7 +8197,7 @@
     </row>
     <row r="26" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A26" s="64" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B26" s="65" t="s">
         <v>52</v>
@@ -8288,7 +8274,7 @@
     </row>
     <row r="27" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A27" s="64" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B27" s="65" t="s">
         <v>52</v>
@@ -8365,7 +8351,7 @@
     </row>
     <row r="28" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A28" s="64" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B28" s="65" t="s">
         <v>52</v>
@@ -8442,7 +8428,7 @@
     </row>
     <row r="29" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A29" s="64" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B29" s="65" t="s">
         <v>52</v>
@@ -8519,7 +8505,7 @@
     </row>
     <row r="30" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A30" s="64" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B30" s="65" t="s">
         <v>52</v>
@@ -8596,7 +8582,7 @@
     </row>
     <row r="31" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A31" s="64" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B31" s="65" t="s">
         <v>52</v>
@@ -8673,7 +8659,7 @@
     </row>
     <row r="32" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A32" s="64" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B32" s="65" t="s">
         <v>52</v>
@@ -8750,7 +8736,7 @@
     </row>
     <row r="33" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A33" s="64" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B33" s="65" t="s">
         <v>52</v>
@@ -8827,10 +8813,10 @@
     </row>
     <row r="34" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A34" s="64" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B34" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C34" s="37" t="s">
         <v>53</v>
@@ -8904,10 +8890,10 @@
     </row>
     <row r="35" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A35" s="64" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B35" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C35" s="37" t="s">
         <v>53</v>
@@ -8981,10 +8967,10 @@
     </row>
     <row r="36" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A36" s="64" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B36" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C36" s="37" t="s">
         <v>53</v>
@@ -9058,10 +9044,10 @@
     </row>
     <row r="37" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A37" s="64" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B37" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C37" s="37" t="s">
         <v>53</v>
@@ -9135,10 +9121,10 @@
     </row>
     <row r="38" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A38" s="64" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B38" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C38" s="37" t="s">
         <v>53</v>
@@ -9212,10 +9198,10 @@
     </row>
     <row r="39" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A39" s="64" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B39" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C39" s="37" t="s">
         <v>53</v>
@@ -9289,10 +9275,10 @@
     </row>
     <row r="40" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A40" s="64" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B40" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C40" s="37" t="s">
         <v>53</v>
@@ -9366,10 +9352,10 @@
     </row>
     <row r="41" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A41" s="64" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B41" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C41" s="37" t="s">
         <v>53</v>
@@ -9443,10 +9429,10 @@
     </row>
     <row r="42" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A42" s="64" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B42" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C42" s="37" t="s">
         <v>53</v>
@@ -9520,10 +9506,10 @@
     </row>
     <row r="43" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A43" s="64" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B43" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C43" s="37" t="s">
         <v>53</v>
@@ -9597,10 +9583,10 @@
     </row>
     <row r="44" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A44" s="64" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B44" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C44" s="37" t="s">
         <v>53</v>
@@ -9674,10 +9660,10 @@
     </row>
     <row r="45" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A45" s="64" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B45" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C45" s="37" t="s">
         <v>53</v>
@@ -9751,10 +9737,10 @@
     </row>
     <row r="46" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A46" s="64" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B46" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C46" s="37" t="s">
         <v>53</v>
@@ -9828,10 +9814,10 @@
     </row>
     <row r="47" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A47" s="64" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B47" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C47" s="37" t="s">
         <v>53</v>
@@ -9905,10 +9891,10 @@
     </row>
     <row r="48" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A48" s="64" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B48" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C48" s="37" t="s">
         <v>53</v>
@@ -9982,10 +9968,10 @@
     </row>
     <row r="49" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A49" s="64" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B49" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C49" s="37" t="s">
         <v>53</v>
@@ -10059,10 +10045,10 @@
     </row>
     <row r="50" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A50" s="64" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B50" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C50" s="37" t="s">
         <v>53</v>
@@ -10136,10 +10122,10 @@
     </row>
     <row r="51" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A51" s="64" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B51" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C51" s="37" t="s">
         <v>53</v>
@@ -10213,10 +10199,10 @@
     </row>
     <row r="52" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A52" s="64" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B52" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C52" s="37" t="s">
         <v>53</v>
@@ -10290,10 +10276,10 @@
     </row>
     <row r="53" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A53" s="64" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B53" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C53" s="37" t="s">
         <v>53</v>
@@ -10367,10 +10353,10 @@
     </row>
     <row r="54" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A54" s="64" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B54" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C54" s="37" t="s">
         <v>53</v>
@@ -10444,10 +10430,10 @@
     </row>
     <row r="55" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A55" s="64" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B55" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C55" s="37" t="s">
         <v>53</v>
@@ -10521,10 +10507,10 @@
     </row>
     <row r="56" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A56" s="64" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B56" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C56" s="37" t="s">
         <v>53</v>
@@ -10598,10 +10584,10 @@
     </row>
     <row r="57" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A57" s="64" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B57" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C57" s="37" t="s">
         <v>53</v>
@@ -10675,10 +10661,10 @@
     </row>
     <row r="58" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A58" s="64" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B58" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C58" s="37" t="s">
         <v>53</v>
@@ -10752,10 +10738,10 @@
     </row>
     <row r="59" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A59" s="64" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B59" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C59" s="37" t="s">
         <v>53</v>
@@ -10829,10 +10815,10 @@
     </row>
     <row r="60" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A60" s="64" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B60" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C60" s="37" t="s">
         <v>53</v>
@@ -10906,10 +10892,10 @@
     </row>
     <row r="61" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A61" s="64" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B61" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C61" s="37" t="s">
         <v>53</v>
@@ -10983,10 +10969,10 @@
     </row>
     <row r="62" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A62" s="64" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B62" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C62" s="37" t="s">
         <v>53</v>
@@ -11060,10 +11046,10 @@
     </row>
     <row r="63" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A63" s="64" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B63" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C63" s="37" t="s">
         <v>53</v>
@@ -11137,10 +11123,10 @@
     </row>
     <row r="64" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A64" s="64" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B64" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C64" s="37" t="s">
         <v>53</v>
@@ -11214,10 +11200,10 @@
     </row>
     <row r="65" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A65" s="64" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B65" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C65" s="37" t="s">
         <v>53</v>
@@ -11291,10 +11277,10 @@
     </row>
     <row r="66" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A66" s="64" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B66" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C66" s="37" t="s">
         <v>53</v>
@@ -11368,10 +11354,10 @@
     </row>
     <row r="67" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A67" s="64" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B67" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C67" s="37" t="s">
         <v>53</v>
@@ -11445,10 +11431,10 @@
     </row>
     <row r="68" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A68" s="64" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B68" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C68" s="37" t="s">
         <v>53</v>
@@ -11522,10 +11508,10 @@
     </row>
     <row r="69" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A69" s="64" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B69" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C69" s="37" t="s">
         <v>53</v>
@@ -11599,10 +11585,10 @@
     </row>
     <row r="70" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A70" s="64" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B70" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C70" s="37" t="s">
         <v>53</v>
@@ -11676,10 +11662,10 @@
     </row>
     <row r="71" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A71" s="64" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B71" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C71" s="37" t="s">
         <v>53</v>
@@ -11753,10 +11739,10 @@
     </row>
     <row r="72" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A72" s="64" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B72" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C72" s="37" t="s">
         <v>53</v>
@@ -11830,10 +11816,10 @@
     </row>
     <row r="73" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A73" s="64" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B73" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C73" s="37" t="s">
         <v>53</v>
@@ -11907,7 +11893,7 @@
     </row>
     <row r="74" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A74" s="64" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B74" s="65" t="s">
         <v>52</v>
@@ -11984,7 +11970,7 @@
     </row>
     <row r="75" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A75" s="64" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B75" s="65" t="s">
         <v>52</v>
@@ -12061,7 +12047,7 @@
     </row>
     <row r="76" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A76" s="64" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B76" s="65" t="s">
         <v>52</v>
@@ -12138,7 +12124,7 @@
     </row>
     <row r="77" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A77" s="64" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B77" s="65" t="s">
         <v>52</v>
@@ -12215,7 +12201,7 @@
     </row>
     <row r="78" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A78" s="64" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B78" s="65" t="s">
         <v>52</v>
@@ -12292,7 +12278,7 @@
     </row>
     <row r="79" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A79" s="64" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B79" s="65" t="s">
         <v>52</v>
@@ -12369,7 +12355,7 @@
     </row>
     <row r="80" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A80" s="64" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B80" s="65" t="s">
         <v>52</v>
@@ -12446,7 +12432,7 @@
     </row>
     <row r="81" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A81" s="64" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B81" s="65" t="s">
         <v>52</v>
@@ -12523,7 +12509,7 @@
     </row>
     <row r="82" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A82" s="64" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B82" s="65" t="s">
         <v>52</v>
@@ -12600,7 +12586,7 @@
     </row>
     <row r="83" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A83" s="64" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B83" s="65" t="s">
         <v>52</v>
@@ -12677,7 +12663,7 @@
     </row>
     <row r="84" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A84" s="64" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B84" s="65" t="s">
         <v>52</v>
@@ -12754,7 +12740,7 @@
     </row>
     <row r="85" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A85" s="64" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B85" s="65" t="s">
         <v>52</v>
@@ -12831,7 +12817,7 @@
     </row>
     <row r="86" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A86" s="64" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B86" s="65" t="s">
         <v>52</v>
@@ -12908,7 +12894,7 @@
     </row>
     <row r="87" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A87" s="64" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B87" s="65" t="s">
         <v>52</v>
@@ -12985,7 +12971,7 @@
     </row>
     <row r="88" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A88" s="64" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B88" s="65" t="s">
         <v>52</v>
@@ -13062,7 +13048,7 @@
     </row>
     <row r="89" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A89" s="64" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B89" s="65" t="s">
         <v>52</v>
@@ -13139,7 +13125,7 @@
     </row>
     <row r="90" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A90" s="64" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B90" s="65" t="s">
         <v>52</v>
@@ -13216,7 +13202,7 @@
     </row>
     <row r="91" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A91" s="64" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B91" s="65" t="s">
         <v>52</v>
@@ -13293,7 +13279,7 @@
     </row>
     <row r="92" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A92" s="64" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B92" s="65" t="s">
         <v>52</v>
@@ -13370,7 +13356,7 @@
     </row>
     <row r="93" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A93" s="64" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B93" s="65" t="s">
         <v>52</v>
@@ -13447,7 +13433,7 @@
     </row>
     <row r="94" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A94" s="64" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B94" s="65" t="s">
         <v>52</v>
@@ -13524,7 +13510,7 @@
     </row>
     <row r="95" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A95" s="64" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B95" s="65" t="s">
         <v>52</v>
@@ -13601,7 +13587,7 @@
     </row>
     <row r="96" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A96" s="64" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B96" s="65" t="s">
         <v>52</v>
@@ -13678,7 +13664,7 @@
     </row>
     <row r="97" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A97" s="64" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B97" s="65" t="s">
         <v>52</v>
@@ -13755,7 +13741,7 @@
     </row>
     <row r="98" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A98" s="64" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B98" s="65" t="s">
         <v>52</v>
@@ -13832,7 +13818,7 @@
     </row>
     <row r="99" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A99" s="64" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B99" s="65" t="s">
         <v>52</v>
@@ -13909,7 +13895,7 @@
     </row>
     <row r="100" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A100" s="64" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B100" s="65" t="s">
         <v>52</v>
@@ -13986,7 +13972,7 @@
     </row>
     <row r="101" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A101" s="64" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B101" s="65" t="s">
         <v>52</v>
@@ -14063,7 +14049,7 @@
     </row>
     <row r="102" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A102" s="64" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B102" s="65" t="s">
         <v>52</v>
@@ -14140,7 +14126,7 @@
     </row>
     <row r="103" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A103" s="64" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B103" s="65" t="s">
         <v>52</v>
@@ -14217,7 +14203,7 @@
     </row>
     <row r="104" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A104" s="64" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B104" s="65" t="s">
         <v>52</v>
@@ -14294,7 +14280,7 @@
     </row>
     <row r="105" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A105" s="64" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B105" s="65" t="s">
         <v>52</v>
@@ -14371,7 +14357,7 @@
     </row>
     <row r="106" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A106" s="64" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B106" s="65" t="s">
         <v>52</v>
@@ -14448,7 +14434,7 @@
     </row>
     <row r="107" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A107" s="64" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B107" s="65" t="s">
         <v>52</v>
@@ -14525,7 +14511,7 @@
     </row>
     <row r="108" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A108" s="64" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B108" s="65" t="s">
         <v>52</v>
@@ -14602,7 +14588,7 @@
     </row>
     <row r="109" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A109" s="64" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B109" s="65" t="s">
         <v>52</v>
@@ -14679,7 +14665,7 @@
     </row>
     <row r="110" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A110" s="64" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B110" s="65" t="s">
         <v>52</v>
@@ -14756,7 +14742,7 @@
     </row>
     <row r="111" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A111" s="64" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B111" s="65" t="s">
         <v>52</v>
@@ -14833,7 +14819,7 @@
     </row>
     <row r="112" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A112" s="64" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B112" s="65" t="s">
         <v>52</v>
@@ -14910,7 +14896,7 @@
     </row>
     <row r="113" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A113" s="64" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B113" s="65" t="s">
         <v>52</v>
@@ -14987,7 +14973,7 @@
     </row>
     <row r="114" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A114" s="64" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B114" s="65" t="s">
         <v>52</v>
@@ -15064,7 +15050,7 @@
     </row>
     <row r="115" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A115" s="64" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B115" s="65" t="s">
         <v>52</v>
@@ -15141,7 +15127,7 @@
     </row>
     <row r="116" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A116" s="64" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B116" s="65" t="s">
         <v>52</v>
@@ -15218,7 +15204,7 @@
     </row>
     <row r="117" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A117" s="64" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B117" s="65" t="s">
         <v>52</v>
@@ -15295,7 +15281,7 @@
     </row>
     <row r="118" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A118" s="64" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B118" s="65" t="s">
         <v>52</v>
@@ -15372,7 +15358,7 @@
     </row>
     <row r="119" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A119" s="64" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B119" s="65" t="s">
         <v>52</v>
@@ -15449,7 +15435,7 @@
     </row>
     <row r="120" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A120" s="64" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B120" s="65" t="s">
         <v>52</v>
@@ -15526,7 +15512,7 @@
     </row>
     <row r="121" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A121" s="64" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B121" s="65" t="s">
         <v>52</v>
@@ -15603,7 +15589,7 @@
     </row>
     <row r="122" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A122" s="64" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B122" s="65" t="s">
         <v>52</v>
@@ -15680,7 +15666,7 @@
     </row>
     <row r="123" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A123" s="64" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B123" s="65" t="s">
         <v>52</v>
@@ -15757,7 +15743,7 @@
     </row>
     <row r="124" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A124" s="64" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B124" s="65" t="s">
         <v>52</v>
@@ -15834,7 +15820,7 @@
     </row>
     <row r="125" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A125" s="64" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B125" s="65" t="s">
         <v>52</v>
@@ -15911,7 +15897,7 @@
     </row>
     <row r="126" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A126" s="64" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B126" s="65" t="s">
         <v>52</v>
@@ -15988,7 +15974,7 @@
     </row>
     <row r="127" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A127" s="64" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B127" s="65" t="s">
         <v>52</v>
@@ -16065,7 +16051,7 @@
     </row>
     <row r="128" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A128" s="64" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B128" s="65" t="s">
         <v>52</v>
@@ -16142,7 +16128,7 @@
     </row>
     <row r="129" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A129" s="64" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B129" s="65" t="s">
         <v>52</v>
@@ -16219,7 +16205,7 @@
     </row>
     <row r="130" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A130" s="64" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B130" s="65" t="s">
         <v>52</v>
@@ -16296,7 +16282,7 @@
     </row>
     <row r="131" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A131" s="64" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B131" s="65" t="s">
         <v>52</v>
@@ -16373,7 +16359,7 @@
     </row>
     <row r="132" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A132" s="64" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B132" s="65" t="s">
         <v>52</v>
@@ -16450,7 +16436,7 @@
     </row>
     <row r="133" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A133" s="64" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B133" s="65" t="s">
         <v>52</v>
@@ -16527,10 +16513,10 @@
     </row>
     <row r="134" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A134" s="64" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B134" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C134" s="37" t="s">
         <v>53</v>
@@ -16604,10 +16590,10 @@
     </row>
     <row r="135" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A135" s="64" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B135" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C135" s="37" t="s">
         <v>53</v>
@@ -16681,10 +16667,10 @@
     </row>
     <row r="136" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A136" s="64" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B136" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C136" s="37" t="s">
         <v>53</v>
@@ -16758,10 +16744,10 @@
     </row>
     <row r="137" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A137" s="64" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B137" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C137" s="37" t="s">
         <v>53</v>
@@ -16835,10 +16821,10 @@
     </row>
     <row r="138" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A138" s="64" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B138" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C138" s="37" t="s">
         <v>53</v>
@@ -16912,10 +16898,10 @@
     </row>
     <row r="139" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A139" s="64" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B139" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C139" s="37" t="s">
         <v>53</v>
@@ -16989,10 +16975,10 @@
     </row>
     <row r="140" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A140" s="64" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B140" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C140" s="37" t="s">
         <v>53</v>
@@ -17066,10 +17052,10 @@
     </row>
     <row r="141" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A141" s="64" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B141" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C141" s="37" t="s">
         <v>53</v>
@@ -17143,10 +17129,10 @@
     </row>
     <row r="142" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A142" s="64" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B142" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C142" s="37" t="s">
         <v>53</v>
@@ -17220,10 +17206,10 @@
     </row>
     <row r="143" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A143" s="64" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B143" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C143" s="37" t="s">
         <v>53</v>
@@ -17297,10 +17283,10 @@
     </row>
     <row r="144" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A144" s="64" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B144" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C144" s="37" t="s">
         <v>53</v>
@@ -17374,10 +17360,10 @@
     </row>
     <row r="145" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A145" s="64" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B145" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C145" s="37" t="s">
         <v>53</v>
@@ -17451,10 +17437,10 @@
     </row>
     <row r="146" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A146" s="64" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B146" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C146" s="37" t="s">
         <v>53</v>
@@ -17528,10 +17514,10 @@
     </row>
     <row r="147" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A147" s="64" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B147" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C147" s="37" t="s">
         <v>53</v>
@@ -17605,10 +17591,10 @@
     </row>
     <row r="148" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A148" s="64" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B148" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C148" s="37" t="s">
         <v>53</v>
@@ -17682,10 +17668,10 @@
     </row>
     <row r="149" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A149" s="64" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B149" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C149" s="37" t="s">
         <v>53</v>
@@ -17759,10 +17745,10 @@
     </row>
     <row r="150" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A150" s="64" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B150" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C150" s="37" t="s">
         <v>53</v>
@@ -17836,10 +17822,10 @@
     </row>
     <row r="151" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A151" s="64" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B151" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C151" s="37" t="s">
         <v>53</v>
@@ -17913,10 +17899,10 @@
     </row>
     <row r="152" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A152" s="64" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B152" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C152" s="37" t="s">
         <v>53</v>
@@ -17990,10 +17976,10 @@
     </row>
     <row r="153" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A153" s="64" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B153" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C153" s="37" t="s">
         <v>53</v>
@@ -18067,10 +18053,10 @@
     </row>
     <row r="154" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A154" s="64" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B154" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C154" s="37" t="s">
         <v>53</v>
@@ -18144,10 +18130,10 @@
     </row>
     <row r="155" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A155" s="64" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B155" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C155" s="37" t="s">
         <v>53</v>
@@ -18221,10 +18207,10 @@
     </row>
     <row r="156" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A156" s="64" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B156" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C156" s="37" t="s">
         <v>53</v>
@@ -18298,10 +18284,10 @@
     </row>
     <row r="157" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A157" s="64" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B157" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C157" s="37" t="s">
         <v>53</v>
@@ -18375,10 +18361,10 @@
     </row>
     <row r="158" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A158" s="64" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B158" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C158" s="37" t="s">
         <v>53</v>
@@ -18452,10 +18438,10 @@
     </row>
     <row r="159" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A159" s="64" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B159" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C159" s="37" t="s">
         <v>53</v>
@@ -18529,10 +18515,10 @@
     </row>
     <row r="160" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A160" s="64" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B160" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C160" s="37" t="s">
         <v>53</v>
@@ -18606,10 +18592,10 @@
     </row>
     <row r="161" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A161" s="64" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B161" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C161" s="37" t="s">
         <v>53</v>
@@ -18683,10 +18669,10 @@
     </row>
     <row r="162" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A162" s="64" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B162" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C162" s="37" t="s">
         <v>53</v>
@@ -18760,10 +18746,10 @@
     </row>
     <row r="163" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A163" s="64" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B163" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C163" s="37" t="s">
         <v>53</v>
@@ -18837,10 +18823,10 @@
     </row>
     <row r="164" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A164" s="64" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B164" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C164" s="37" t="s">
         <v>53</v>
@@ -18914,10 +18900,10 @@
     </row>
     <row r="165" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A165" s="64" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B165" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C165" s="37" t="s">
         <v>53</v>
@@ -18991,10 +18977,10 @@
     </row>
     <row r="166" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A166" s="64" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B166" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C166" s="37" t="s">
         <v>53</v>
@@ -19068,10 +19054,10 @@
     </row>
     <row r="167" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A167" s="64" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B167" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C167" s="37" t="s">
         <v>53</v>
@@ -19145,10 +19131,10 @@
     </row>
     <row r="168" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A168" s="64" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B168" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C168" s="37" t="s">
         <v>53</v>
@@ -19222,10 +19208,10 @@
     </row>
     <row r="169" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A169" s="64" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B169" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C169" s="37" t="s">
         <v>53</v>
@@ -19299,10 +19285,10 @@
     </row>
     <row r="170" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A170" s="64" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B170" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C170" s="37" t="s">
         <v>53</v>
@@ -19376,10 +19362,10 @@
     </row>
     <row r="171" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A171" s="64" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B171" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C171" s="37" t="s">
         <v>53</v>
@@ -19453,10 +19439,10 @@
     </row>
     <row r="172" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A172" s="64" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B172" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C172" s="37" t="s">
         <v>53</v>
@@ -19530,10 +19516,10 @@
     </row>
     <row r="173" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A173" s="64" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B173" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C173" s="37" t="s">
         <v>53</v>
@@ -19607,7 +19593,7 @@
     </row>
     <row r="174" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A174" s="64" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B174" s="65" t="s">
         <v>52</v>
@@ -19684,7 +19670,7 @@
     </row>
     <row r="175" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A175" s="64" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B175" s="65" t="s">
         <v>52</v>
@@ -19761,7 +19747,7 @@
     </row>
     <row r="176" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A176" s="64" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B176" s="65" t="s">
         <v>52</v>
@@ -19838,7 +19824,7 @@
     </row>
     <row r="177" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A177" s="64" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B177" s="65" t="s">
         <v>52</v>
@@ -19915,7 +19901,7 @@
     </row>
     <row r="178" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A178" s="64" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B178" s="65" t="s">
         <v>52</v>
@@ -19992,7 +19978,7 @@
     </row>
     <row r="179" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A179" s="64" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B179" s="65" t="s">
         <v>52</v>
@@ -20069,7 +20055,7 @@
     </row>
     <row r="180" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A180" s="64" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B180" s="65" t="s">
         <v>52</v>
@@ -20146,7 +20132,7 @@
     </row>
     <row r="181" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A181" s="64" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B181" s="65" t="s">
         <v>52</v>
@@ -20223,7 +20209,7 @@
     </row>
     <row r="182" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A182" s="64" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B182" s="65" t="s">
         <v>52</v>
@@ -20300,7 +20286,7 @@
     </row>
     <row r="183" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A183" s="64" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B183" s="65" t="s">
         <v>52</v>
@@ -20377,7 +20363,7 @@
     </row>
     <row r="184" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A184" s="64" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B184" s="65" t="s">
         <v>52</v>
@@ -20454,7 +20440,7 @@
     </row>
     <row r="185" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A185" s="64" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B185" s="65" t="s">
         <v>52</v>
@@ -20531,7 +20517,7 @@
     </row>
     <row r="186" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A186" s="64" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B186" s="65" t="s">
         <v>52</v>
@@ -20608,7 +20594,7 @@
     </row>
     <row r="187" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A187" s="64" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B187" s="65" t="s">
         <v>52</v>
@@ -20685,7 +20671,7 @@
     </row>
     <row r="188" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A188" s="64" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B188" s="65" t="s">
         <v>52</v>
@@ -20762,7 +20748,7 @@
     </row>
     <row r="189" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A189" s="64" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B189" s="65" t="s">
         <v>52</v>
@@ -20839,7 +20825,7 @@
     </row>
     <row r="190" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A190" s="64" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B190" s="65" t="s">
         <v>52</v>
@@ -20916,7 +20902,7 @@
     </row>
     <row r="191" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A191" s="64" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B191" s="65" t="s">
         <v>52</v>
@@ -20993,7 +20979,7 @@
     </row>
     <row r="192" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A192" s="64" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B192" s="65" t="s">
         <v>52</v>
@@ -21070,7 +21056,7 @@
     </row>
     <row r="193" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A193" s="64" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B193" s="65" t="s">
         <v>52</v>
@@ -21147,7 +21133,7 @@
     </row>
     <row r="194" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A194" s="64" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B194" s="65" t="s">
         <v>52</v>
@@ -21224,7 +21210,7 @@
     </row>
     <row r="195" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A195" s="64" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B195" s="65" t="s">
         <v>52</v>
@@ -21301,7 +21287,7 @@
     </row>
     <row r="196" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A196" s="64" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B196" s="65" t="s">
         <v>52</v>
@@ -21378,7 +21364,7 @@
     </row>
     <row r="197" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A197" s="64" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B197" s="65" t="s">
         <v>52</v>
@@ -21455,7 +21441,7 @@
     </row>
     <row r="198" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A198" s="64" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B198" s="65" t="s">
         <v>52</v>
@@ -21532,7 +21518,7 @@
     </row>
     <row r="199" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A199" s="64" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B199" s="65" t="s">
         <v>52</v>
@@ -21609,7 +21595,7 @@
     </row>
     <row r="200" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A200" s="64" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B200" s="65" t="s">
         <v>52</v>
@@ -21686,7 +21672,7 @@
     </row>
     <row r="201" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A201" s="64" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B201" s="65" t="s">
         <v>52</v>
@@ -21763,7 +21749,7 @@
     </row>
     <row r="202" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A202" s="64" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B202" s="65" t="s">
         <v>52</v>
@@ -21840,7 +21826,7 @@
     </row>
     <row r="203" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A203" s="64" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B203" s="65" t="s">
         <v>52</v>
@@ -21917,7 +21903,7 @@
     </row>
     <row r="204" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A204" s="64" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B204" s="65" t="s">
         <v>52</v>
@@ -21994,7 +21980,7 @@
     </row>
     <row r="205" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A205" s="64" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B205" s="65" t="s">
         <v>52</v>
@@ -22071,7 +22057,7 @@
     </row>
     <row r="206" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A206" s="64" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B206" s="65" t="s">
         <v>52</v>
@@ -22148,7 +22134,7 @@
     </row>
     <row r="207" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A207" s="64" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B207" s="65" t="s">
         <v>52</v>
@@ -22225,7 +22211,7 @@
     </row>
     <row r="208" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A208" s="64" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B208" s="65" t="s">
         <v>52</v>
@@ -22302,7 +22288,7 @@
     </row>
     <row r="209" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A209" s="64" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B209" s="65" t="s">
         <v>52</v>
@@ -22379,7 +22365,7 @@
     </row>
     <row r="210" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A210" s="64" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B210" s="65" t="s">
         <v>52</v>
@@ -22456,7 +22442,7 @@
     </row>
     <row r="211" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A211" s="64" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B211" s="65" t="s">
         <v>52</v>
@@ -22533,7 +22519,7 @@
     </row>
     <row r="212" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A212" s="64" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B212" s="65" t="s">
         <v>52</v>
@@ -22610,7 +22596,7 @@
     </row>
     <row r="213" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A213" s="64" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B213" s="65" t="s">
         <v>52</v>
@@ -22687,7 +22673,7 @@
     </row>
     <row r="214" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A214" s="64" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B214" s="65" t="s">
         <v>52</v>
@@ -22764,7 +22750,7 @@
     </row>
     <row r="215" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A215" s="64" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B215" s="65" t="s">
         <v>52</v>
@@ -22841,7 +22827,7 @@
     </row>
     <row r="216" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A216" s="64" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B216" s="65" t="s">
         <v>52</v>
@@ -22918,7 +22904,7 @@
     </row>
     <row r="217" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A217" s="64" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B217" s="65" t="s">
         <v>52</v>
@@ -22995,7 +22981,7 @@
     </row>
     <row r="218" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A218" s="64" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B218" s="65" t="s">
         <v>52</v>
@@ -23072,7 +23058,7 @@
     </row>
     <row r="219" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A219" s="64" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B219" s="65" t="s">
         <v>52</v>
@@ -23149,7 +23135,7 @@
     </row>
     <row r="220" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A220" s="64" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B220" s="65" t="s">
         <v>52</v>
@@ -23226,7 +23212,7 @@
     </row>
     <row r="221" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A221" s="64" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B221" s="65" t="s">
         <v>52</v>
@@ -23303,7 +23289,7 @@
     </row>
     <row r="222" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A222" s="64" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B222" s="65" t="s">
         <v>52</v>
@@ -23380,7 +23366,7 @@
     </row>
     <row r="223" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A223" s="64" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B223" s="65" t="s">
         <v>52</v>
@@ -23457,7 +23443,7 @@
     </row>
     <row r="224" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A224" s="64" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B224" s="65" t="s">
         <v>52</v>
@@ -23534,7 +23520,7 @@
     </row>
     <row r="225" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A225" s="64" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B225" s="65" t="s">
         <v>52</v>
@@ -23611,7 +23597,7 @@
     </row>
     <row r="226" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A226" s="64" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B226" s="65" t="s">
         <v>52</v>
@@ -23688,7 +23674,7 @@
     </row>
     <row r="227" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A227" s="64" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B227" s="65" t="s">
         <v>52</v>
@@ -23765,7 +23751,7 @@
     </row>
     <row r="228" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A228" s="64" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B228" s="65" t="s">
         <v>52</v>
@@ -23842,7 +23828,7 @@
     </row>
     <row r="229" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A229" s="64" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B229" s="65" t="s">
         <v>52</v>
@@ -23919,7 +23905,7 @@
     </row>
     <row r="230" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A230" s="64" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B230" s="65" t="s">
         <v>52</v>
@@ -23996,7 +23982,7 @@
     </row>
     <row r="231" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A231" s="64" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B231" s="65" t="s">
         <v>52</v>
@@ -24073,7 +24059,7 @@
     </row>
     <row r="232" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A232" s="64" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B232" s="65" t="s">
         <v>52</v>
@@ -24150,7 +24136,7 @@
     </row>
     <row r="233" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A233" s="64" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B233" s="65" t="s">
         <v>52</v>
@@ -24227,7 +24213,7 @@
     </row>
     <row r="234" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A234" s="64" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B234" s="65" t="s">
         <v>52</v>
@@ -24304,7 +24290,7 @@
     </row>
     <row r="235" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A235" s="64" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B235" s="65" t="s">
         <v>52</v>
@@ -24381,7 +24367,7 @@
     </row>
     <row r="236" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A236" s="64" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B236" s="65" t="s">
         <v>52</v>
@@ -24458,7 +24444,7 @@
     </row>
     <row r="237" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A237" s="64" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B237" s="65" t="s">
         <v>52</v>
@@ -24535,7 +24521,7 @@
     </row>
     <row r="238" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A238" s="64" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B238" s="65" t="s">
         <v>52</v>
@@ -24612,7 +24598,7 @@
     </row>
     <row r="239" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A239" s="64" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B239" s="65" t="s">
         <v>52</v>
@@ -24689,7 +24675,7 @@
     </row>
     <row r="240" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A240" s="64" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B240" s="65" t="s">
         <v>52</v>
@@ -24766,7 +24752,7 @@
     </row>
     <row r="241" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A241" s="64" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B241" s="65" t="s">
         <v>52</v>
@@ -24843,7 +24829,7 @@
     </row>
     <row r="242" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A242" s="64" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B242" s="65" t="s">
         <v>52</v>
@@ -24920,7 +24906,7 @@
     </row>
     <row r="243" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A243" s="64" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B243" s="65" t="s">
         <v>52</v>
@@ -24997,7 +24983,7 @@
     </row>
     <row r="244" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A244" s="64" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B244" s="65" t="s">
         <v>52</v>
@@ -25074,7 +25060,7 @@
     </row>
     <row r="245" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A245" s="64" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B245" s="65" t="s">
         <v>52</v>
@@ -25151,7 +25137,7 @@
     </row>
     <row r="246" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A246" s="64" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B246" s="65" t="s">
         <v>52</v>
@@ -25228,7 +25214,7 @@
     </row>
     <row r="247" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A247" s="64" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B247" s="65" t="s">
         <v>52</v>
@@ -25305,7 +25291,7 @@
     </row>
     <row r="248" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A248" s="64" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B248" s="65" t="s">
         <v>52</v>
@@ -25382,7 +25368,7 @@
     </row>
     <row r="249" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A249" s="64" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B249" s="65" t="s">
         <v>52</v>
@@ -25459,7 +25445,7 @@
     </row>
     <row r="250" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A250" s="64" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B250" s="65" t="s">
         <v>52</v>
@@ -25536,7 +25522,7 @@
     </row>
     <row r="251" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A251" s="64" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B251" s="65" t="s">
         <v>52</v>
@@ -25613,7 +25599,7 @@
     </row>
     <row r="252" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A252" s="64" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B252" s="65" t="s">
         <v>52</v>
@@ -25690,7 +25676,7 @@
     </row>
     <row r="253" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A253" s="64" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B253" s="65" t="s">
         <v>52</v>
@@ -25767,7 +25753,7 @@
     </row>
     <row r="254" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A254" s="64" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B254" s="65" t="s">
         <v>52</v>
@@ -25844,7 +25830,7 @@
     </row>
     <row r="255" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A255" s="64" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B255" s="65" t="s">
         <v>52</v>
@@ -25921,7 +25907,7 @@
     </row>
     <row r="256" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A256" s="64" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B256" s="65" t="s">
         <v>52</v>
@@ -25998,7 +25984,7 @@
     </row>
     <row r="257" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A257" s="64" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B257" s="65" t="s">
         <v>52</v>
@@ -26075,7 +26061,7 @@
     </row>
     <row r="258" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A258" s="64" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B258" s="65" t="s">
         <v>52</v>
@@ -26152,7 +26138,7 @@
     </row>
     <row r="259" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A259" s="64" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B259" s="65" t="s">
         <v>52</v>
@@ -26229,7 +26215,7 @@
     </row>
     <row r="260" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A260" s="64" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B260" s="65" t="s">
         <v>52</v>
@@ -26306,7 +26292,7 @@
     </row>
     <row r="261" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A261" s="64" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B261" s="65" t="s">
         <v>52</v>
@@ -26383,7 +26369,7 @@
     </row>
     <row r="262" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A262" s="64" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B262" s="65" t="s">
         <v>52</v>
@@ -26460,7 +26446,7 @@
     </row>
     <row r="263" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A263" s="64" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B263" s="65" t="s">
         <v>52</v>
@@ -26537,7 +26523,7 @@
     </row>
     <row r="264" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A264" s="64" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B264" s="65" t="s">
         <v>52</v>
@@ -26614,7 +26600,7 @@
     </row>
     <row r="265" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A265" s="64" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B265" s="65" t="s">
         <v>52</v>
@@ -26691,7 +26677,7 @@
     </row>
     <row r="266" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A266" s="64" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B266" s="65" t="s">
         <v>52</v>
@@ -26768,7 +26754,7 @@
     </row>
     <row r="267" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A267" s="64" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B267" s="65" t="s">
         <v>52</v>
@@ -26845,7 +26831,7 @@
     </row>
     <row r="268" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A268" s="64" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B268" s="65" t="s">
         <v>52</v>
@@ -26922,7 +26908,7 @@
     </row>
     <row r="269" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A269" s="64" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B269" s="65" t="s">
         <v>52</v>
@@ -26999,7 +26985,7 @@
     </row>
     <row r="270" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A270" s="64" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B270" s="65" t="s">
         <v>52</v>
@@ -27076,7 +27062,7 @@
     </row>
     <row r="271" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A271" s="64" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B271" s="65" t="s">
         <v>52</v>
@@ -27153,7 +27139,7 @@
     </row>
     <row r="272" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A272" s="64" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B272" s="65" t="s">
         <v>52</v>
@@ -27230,7 +27216,7 @@
     </row>
     <row r="273" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A273" s="64" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B273" s="65" t="s">
         <v>52</v>
@@ -27307,10 +27293,10 @@
     </row>
     <row r="274" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A274" s="64" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B274" s="66" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C274" s="37" t="s">
         <v>53</v>
@@ -27384,10 +27370,10 @@
     </row>
     <row r="275" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A275" s="64" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B275" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C275" s="37" t="s">
         <v>53</v>
@@ -27461,10 +27447,10 @@
     </row>
     <row r="276" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A276" s="64" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B276" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C276" s="37" t="s">
         <v>53</v>
@@ -27538,10 +27524,10 @@
     </row>
     <row r="277" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A277" s="64" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B277" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C277" s="37" t="s">
         <v>53</v>
@@ -27615,10 +27601,10 @@
     </row>
     <row r="278" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A278" s="64" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B278" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C278" s="37" t="s">
         <v>53</v>
@@ -27692,10 +27678,10 @@
     </row>
     <row r="279" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A279" s="64" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B279" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C279" s="37" t="s">
         <v>53</v>
@@ -27769,10 +27755,10 @@
     </row>
     <row r="280" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A280" s="64" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B280" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C280" s="37" t="s">
         <v>53</v>
@@ -27846,10 +27832,10 @@
     </row>
     <row r="281" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A281" s="64" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B281" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C281" s="37" t="s">
         <v>53</v>
@@ -27923,10 +27909,10 @@
     </row>
     <row r="282" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A282" s="64" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B282" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C282" s="37" t="s">
         <v>53</v>
@@ -28000,10 +27986,10 @@
     </row>
     <row r="283" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A283" s="64" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B283" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C283" s="37" t="s">
         <v>53</v>
@@ -28077,10 +28063,10 @@
     </row>
     <row r="284" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A284" s="64" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B284" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C284" s="37" t="s">
         <v>53</v>
@@ -28154,10 +28140,10 @@
     </row>
     <row r="285" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A285" s="64" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B285" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C285" s="37" t="s">
         <v>53</v>
@@ -28231,10 +28217,10 @@
     </row>
     <row r="286" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A286" s="64" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B286" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C286" s="37" t="s">
         <v>53</v>
@@ -28308,10 +28294,10 @@
     </row>
     <row r="287" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A287" s="64" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B287" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C287" s="37" t="s">
         <v>53</v>
@@ -28385,10 +28371,10 @@
     </row>
     <row r="288" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A288" s="64" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B288" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C288" s="37" t="s">
         <v>53</v>
@@ -28462,10 +28448,10 @@
     </row>
     <row r="289" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A289" s="64" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B289" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C289" s="37" t="s">
         <v>53</v>
@@ -28539,10 +28525,10 @@
     </row>
     <row r="290" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A290" s="64" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B290" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C290" s="37" t="s">
         <v>53</v>
@@ -28616,10 +28602,10 @@
     </row>
     <row r="291" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A291" s="64" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B291" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C291" s="37" t="s">
         <v>53</v>
@@ -28693,10 +28679,10 @@
     </row>
     <row r="292" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A292" s="64" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B292" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C292" s="37" t="s">
         <v>53</v>
@@ -28770,10 +28756,10 @@
     </row>
     <row r="293" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A293" s="64" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B293" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C293" s="37" t="s">
         <v>53</v>
@@ -28847,10 +28833,10 @@
     </row>
     <row r="294" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A294" s="64" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B294" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C294" s="37" t="s">
         <v>53</v>
@@ -28924,10 +28910,10 @@
     </row>
     <row r="295" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A295" s="64" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B295" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C295" s="37" t="s">
         <v>53</v>
@@ -29001,10 +28987,10 @@
     </row>
     <row r="296" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A296" s="64" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B296" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C296" s="37" t="s">
         <v>53</v>
@@ -29078,10 +29064,10 @@
     </row>
     <row r="297" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A297" s="64" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B297" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C297" s="37" t="s">
         <v>53</v>
@@ -29155,10 +29141,10 @@
     </row>
     <row r="298" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A298" s="64" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B298" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C298" s="37" t="s">
         <v>53</v>
@@ -29232,10 +29218,10 @@
     </row>
     <row r="299" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A299" s="64" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B299" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C299" s="37" t="s">
         <v>53</v>
@@ -29309,10 +29295,10 @@
     </row>
     <row r="300" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A300" s="64" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B300" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C300" s="37" t="s">
         <v>53</v>
@@ -29386,10 +29372,10 @@
     </row>
     <row r="301" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A301" s="64" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B301" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C301" s="37" t="s">
         <v>53</v>
@@ -29463,10 +29449,10 @@
     </row>
     <row r="302" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A302" s="64" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B302" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C302" s="37" t="s">
         <v>53</v>
@@ -29540,10 +29526,10 @@
     </row>
     <row r="303" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A303" s="64" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B303" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C303" s="37" t="s">
         <v>53</v>
@@ -29617,10 +29603,10 @@
     </row>
     <row r="304" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A304" s="64" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B304" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C304" s="37" t="s">
         <v>53</v>
@@ -29694,10 +29680,10 @@
     </row>
     <row r="305" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A305" s="64" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B305" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C305" s="37" t="s">
         <v>53</v>
@@ -29771,10 +29757,10 @@
     </row>
     <row r="306" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A306" s="64" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B306" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C306" s="37" t="s">
         <v>53</v>
@@ -29848,10 +29834,10 @@
     </row>
     <row r="307" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A307" s="64" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B307" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C307" s="37" t="s">
         <v>53</v>
@@ -29925,10 +29911,10 @@
     </row>
     <row r="308" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A308" s="64" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B308" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C308" s="37" t="s">
         <v>53</v>
@@ -30002,10 +29988,10 @@
     </row>
     <row r="309" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A309" s="64" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B309" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C309" s="37" t="s">
         <v>53</v>
@@ -30079,10 +30065,10 @@
     </row>
     <row r="310" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A310" s="64" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B310" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C310" s="37" t="s">
         <v>53</v>
@@ -30156,10 +30142,10 @@
     </row>
     <row r="311" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A311" s="64" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B311" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C311" s="37" t="s">
         <v>53</v>
@@ -30233,10 +30219,10 @@
     </row>
     <row r="312" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A312" s="64" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B312" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C312" s="37" t="s">
         <v>53</v>
@@ -30310,10 +30296,10 @@
     </row>
     <row r="313" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A313" s="64" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B313" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C313" s="37" t="s">
         <v>53</v>
@@ -30387,10 +30373,10 @@
     </row>
     <row r="314" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A314" s="64" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B314" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C314" s="37" t="s">
         <v>53</v>
@@ -30464,10 +30450,10 @@
     </row>
     <row r="315" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A315" s="64" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B315" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C315" s="37" t="s">
         <v>53</v>
@@ -30541,10 +30527,10 @@
     </row>
     <row r="316" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A316" s="64" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B316" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C316" s="37" t="s">
         <v>53</v>
@@ -30618,10 +30604,10 @@
     </row>
     <row r="317" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A317" s="64" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B317" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C317" s="37" t="s">
         <v>53</v>
@@ -30695,10 +30681,10 @@
     </row>
     <row r="318" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A318" s="64" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B318" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C318" s="37" t="s">
         <v>53</v>
@@ -30772,10 +30758,10 @@
     </row>
     <row r="319" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A319" s="64" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B319" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C319" s="37" t="s">
         <v>53</v>
@@ -30849,10 +30835,10 @@
     </row>
     <row r="320" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A320" s="64" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B320" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C320" s="37" t="s">
         <v>53</v>
@@ -30926,10 +30912,10 @@
     </row>
     <row r="321" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A321" s="64" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B321" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C321" s="37" t="s">
         <v>53</v>
@@ -31003,10 +30989,10 @@
     </row>
     <row r="322" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A322" s="64" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B322" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C322" s="37" t="s">
         <v>53</v>
@@ -31080,10 +31066,10 @@
     </row>
     <row r="323" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A323" s="64" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B323" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C323" s="37" t="s">
         <v>53</v>
@@ -31157,10 +31143,10 @@
     </row>
     <row r="324" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A324" s="64" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B324" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C324" s="37" t="s">
         <v>53</v>
@@ -31234,10 +31220,10 @@
     </row>
     <row r="325" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A325" s="64" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B325" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C325" s="37" t="s">
         <v>53</v>
@@ -31311,10 +31297,10 @@
     </row>
     <row r="326" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A326" s="64" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B326" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C326" s="37" t="s">
         <v>53</v>
@@ -31388,10 +31374,10 @@
     </row>
     <row r="327" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A327" s="64" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B327" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C327" s="37" t="s">
         <v>53</v>
@@ -31465,10 +31451,10 @@
     </row>
     <row r="328" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A328" s="64" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B328" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C328" s="37" t="s">
         <v>53</v>
@@ -31542,10 +31528,10 @@
     </row>
     <row r="329" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A329" s="64" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B329" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C329" s="37" t="s">
         <v>53</v>
@@ -31619,10 +31605,10 @@
     </row>
     <row r="330" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A330" s="64" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B330" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C330" s="37" t="s">
         <v>53</v>
@@ -31696,10 +31682,10 @@
     </row>
     <row r="331" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A331" s="64" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B331" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C331" s="37" t="s">
         <v>53</v>
@@ -31773,10 +31759,10 @@
     </row>
     <row r="332" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A332" s="64" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B332" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C332" s="37" t="s">
         <v>53</v>
@@ -31850,10 +31836,10 @@
     </row>
     <row r="333" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A333" s="64" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B333" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C333" s="37" t="s">
         <v>53</v>
@@ -31927,7 +31913,7 @@
     </row>
     <row r="334" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A334" s="64" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B334" s="65" t="s">
         <v>52</v>
@@ -32004,7 +31990,7 @@
     </row>
     <row r="335" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A335" s="64" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B335" s="65" t="s">
         <v>52</v>
@@ -32081,7 +32067,7 @@
     </row>
     <row r="336" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A336" s="64" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B336" s="65" t="s">
         <v>52</v>
@@ -32158,7 +32144,7 @@
     </row>
     <row r="337" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A337" s="64" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B337" s="65" t="s">
         <v>52</v>
@@ -32235,7 +32221,7 @@
     </row>
     <row r="338" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A338" s="64" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B338" s="65" t="s">
         <v>52</v>
@@ -32312,7 +32298,7 @@
     </row>
     <row r="339" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A339" s="64" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B339" s="65" t="s">
         <v>52</v>
@@ -32389,7 +32375,7 @@
     </row>
     <row r="340" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A340" s="64" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B340" s="65" t="s">
         <v>52</v>
@@ -32466,7 +32452,7 @@
     </row>
     <row r="341" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A341" s="64" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B341" s="65" t="s">
         <v>52</v>
@@ -32543,7 +32529,7 @@
     </row>
     <row r="342" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A342" s="64" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B342" s="65" t="s">
         <v>52</v>
@@ -32620,7 +32606,7 @@
     </row>
     <row r="343" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A343" s="64" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B343" s="65" t="s">
         <v>52</v>
@@ -32697,7 +32683,7 @@
     </row>
     <row r="344" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A344" s="64" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B344" s="65" t="s">
         <v>52</v>
@@ -32774,7 +32760,7 @@
     </row>
     <row r="345" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A345" s="64" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B345" s="65" t="s">
         <v>52</v>
@@ -32851,7 +32837,7 @@
     </row>
     <row r="346" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A346" s="64" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B346" s="65" t="s">
         <v>52</v>
@@ -32928,7 +32914,7 @@
     </row>
     <row r="347" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A347" s="64" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B347" s="65" t="s">
         <v>52</v>
@@ -33005,7 +32991,7 @@
     </row>
     <row r="348" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A348" s="64" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B348" s="65" t="s">
         <v>52</v>
@@ -33082,7 +33068,7 @@
     </row>
     <row r="349" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A349" s="64" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B349" s="65" t="s">
         <v>52</v>
@@ -33159,7 +33145,7 @@
     </row>
     <row r="350" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A350" s="64" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B350" s="65" t="s">
         <v>52</v>
@@ -33236,7 +33222,7 @@
     </row>
     <row r="351" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A351" s="64" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B351" s="65" t="s">
         <v>52</v>
@@ -33313,7 +33299,7 @@
     </row>
     <row r="352" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A352" s="64" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B352" s="65" t="s">
         <v>52</v>
@@ -33390,7 +33376,7 @@
     </row>
     <row r="353" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A353" s="64" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B353" s="65" t="s">
         <v>52</v>
@@ -33467,10 +33453,10 @@
     </row>
     <row r="354" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A354" s="64" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B354" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C354" s="37" t="s">
         <v>53</v>
@@ -33544,10 +33530,10 @@
     </row>
     <row r="355" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A355" s="64" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B355" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C355" s="37" t="s">
         <v>53</v>
@@ -33621,10 +33607,10 @@
     </row>
     <row r="356" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A356" s="64" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B356" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C356" s="37" t="s">
         <v>53</v>
@@ -33698,10 +33684,10 @@
     </row>
     <row r="357" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A357" s="64" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B357" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C357" s="37" t="s">
         <v>53</v>
@@ -33775,10 +33761,10 @@
     </row>
     <row r="358" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A358" s="64" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B358" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C358" s="37" t="s">
         <v>53</v>
@@ -33852,10 +33838,10 @@
     </row>
     <row r="359" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A359" s="64" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B359" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C359" s="37" t="s">
         <v>53</v>
@@ -33929,10 +33915,10 @@
     </row>
     <row r="360" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A360" s="64" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B360" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C360" s="37" t="s">
         <v>53</v>
@@ -34006,10 +33992,10 @@
     </row>
     <row r="361" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A361" s="64" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B361" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C361" s="37" t="s">
         <v>53</v>
@@ -34083,10 +34069,10 @@
     </row>
     <row r="362" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A362" s="64" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B362" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C362" s="37" t="s">
         <v>53</v>
@@ -34160,10 +34146,10 @@
     </row>
     <row r="363" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A363" s="64" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B363" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C363" s="37" t="s">
         <v>53</v>
@@ -34237,10 +34223,10 @@
     </row>
     <row r="364" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A364" s="64" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B364" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C364" s="37" t="s">
         <v>53</v>
@@ -34314,10 +34300,10 @@
     </row>
     <row r="365" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A365" s="64" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B365" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C365" s="37" t="s">
         <v>53</v>
@@ -34391,10 +34377,10 @@
     </row>
     <row r="366" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A366" s="64" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B366" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C366" s="37" t="s">
         <v>53</v>
@@ -34468,10 +34454,10 @@
     </row>
     <row r="367" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A367" s="64" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B367" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C367" s="37" t="s">
         <v>53</v>
@@ -34545,10 +34531,10 @@
     </row>
     <row r="368" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A368" s="64" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B368" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C368" s="37" t="s">
         <v>53</v>
@@ -34622,10 +34608,10 @@
     </row>
     <row r="369" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A369" s="64" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B369" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C369" s="37" t="s">
         <v>53</v>
@@ -34699,10 +34685,10 @@
     </row>
     <row r="370" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A370" s="64" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B370" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C370" s="37" t="s">
         <v>53</v>
@@ -34776,10 +34762,10 @@
     </row>
     <row r="371" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A371" s="64" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B371" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C371" s="37" t="s">
         <v>53</v>
@@ -34853,10 +34839,10 @@
     </row>
     <row r="372" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A372" s="64" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B372" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C372" s="37" t="s">
         <v>53</v>
@@ -34930,10 +34916,10 @@
     </row>
     <row r="373" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A373" s="64" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B373" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C373" s="37" t="s">
         <v>53</v>
@@ -35007,10 +34993,10 @@
     </row>
     <row r="374" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A374" s="64" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B374" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C374" s="37" t="s">
         <v>53</v>
@@ -35084,10 +35070,10 @@
     </row>
     <row r="375" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A375" s="64" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B375" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C375" s="37" t="s">
         <v>53</v>
@@ -35161,10 +35147,10 @@
     </row>
     <row r="376" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A376" s="64" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B376" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C376" s="37" t="s">
         <v>53</v>
@@ -35238,10 +35224,10 @@
     </row>
     <row r="377" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A377" s="64" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B377" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C377" s="37" t="s">
         <v>53</v>
@@ -35315,10 +35301,10 @@
     </row>
     <row r="378" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A378" s="64" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B378" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C378" s="37" t="s">
         <v>53</v>
@@ -35392,10 +35378,10 @@
     </row>
     <row r="379" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A379" s="64" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B379" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C379" s="37" t="s">
         <v>53</v>
@@ -35469,10 +35455,10 @@
     </row>
     <row r="380" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A380" s="64" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B380" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C380" s="37" t="s">
         <v>53</v>
@@ -35546,10 +35532,10 @@
     </row>
     <row r="381" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A381" s="64" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B381" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C381" s="37" t="s">
         <v>53</v>
@@ -35623,10 +35609,10 @@
     </row>
     <row r="382" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A382" s="64" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B382" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C382" s="37" t="s">
         <v>53</v>
@@ -35700,10 +35686,10 @@
     </row>
     <row r="383" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A383" s="64" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B383" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C383" s="37" t="s">
         <v>53</v>
@@ -35777,10 +35763,10 @@
     </row>
     <row r="384" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A384" s="64" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B384" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C384" s="37" t="s">
         <v>53</v>
@@ -35854,10 +35840,10 @@
     </row>
     <row r="385" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A385" s="64" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B385" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C385" s="37" t="s">
         <v>53</v>
@@ -35931,10 +35917,10 @@
     </row>
     <row r="386" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A386" s="64" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B386" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C386" s="37" t="s">
         <v>53</v>
@@ -36008,10 +35994,10 @@
     </row>
     <row r="387" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A387" s="64" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B387" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C387" s="37" t="s">
         <v>53</v>
@@ -36085,10 +36071,10 @@
     </row>
     <row r="388" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A388" s="64" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B388" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C388" s="37" t="s">
         <v>53</v>
@@ -36162,10 +36148,10 @@
     </row>
     <row r="389" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A389" s="64" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B389" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C389" s="37" t="s">
         <v>53</v>
@@ -36239,10 +36225,10 @@
     </row>
     <row r="390" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A390" s="64" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B390" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C390" s="37" t="s">
         <v>53</v>
@@ -36316,10 +36302,10 @@
     </row>
     <row r="391" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A391" s="64" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B391" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C391" s="37" t="s">
         <v>53</v>
@@ -36393,10 +36379,10 @@
     </row>
     <row r="392" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A392" s="64" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B392" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C392" s="37" t="s">
         <v>53</v>
@@ -36470,10 +36456,10 @@
     </row>
     <row r="393" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A393" s="64" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B393" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C393" s="37" t="s">
         <v>53</v>
@@ -36547,10 +36533,10 @@
     </row>
     <row r="394" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A394" s="64" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B394" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C394" s="37" t="s">
         <v>53</v>
@@ -36624,10 +36610,10 @@
     </row>
     <row r="395" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A395" s="64" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B395" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C395" s="37" t="s">
         <v>53</v>
@@ -36701,10 +36687,10 @@
     </row>
     <row r="396" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A396" s="64" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B396" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C396" s="37" t="s">
         <v>53</v>
@@ -36778,10 +36764,10 @@
     </row>
     <row r="397" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A397" s="64" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B397" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C397" s="37" t="s">
         <v>53</v>
@@ -36855,10 +36841,10 @@
     </row>
     <row r="398" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A398" s="64" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B398" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C398" s="37" t="s">
         <v>53</v>
@@ -36932,10 +36918,10 @@
     </row>
     <row r="399" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A399" s="64" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B399" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C399" s="37" t="s">
         <v>53</v>
@@ -37009,10 +36995,10 @@
     </row>
     <row r="400" spans="1:43" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A400" s="64" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B400" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C400" s="37" t="s">
         <v>53</v>
@@ -37086,10 +37072,10 @@
     </row>
     <row r="401" spans="1:23" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A401" s="64" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B401" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C401" s="37" t="s">
         <v>53</v>
@@ -37143,10 +37129,10 @@
     </row>
     <row r="402" spans="1:23" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A402" s="64" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B402" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C402" s="37" t="s">
         <v>53</v>
@@ -37200,10 +37186,10 @@
     </row>
     <row r="403" spans="1:23" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A403" s="64" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B403" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C403" s="37" t="s">
         <v>53</v>
@@ -37257,10 +37243,10 @@
     </row>
     <row r="404" spans="1:23" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A404" s="64" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B404" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C404" s="37" t="s">
         <v>53</v>
@@ -37314,10 +37300,10 @@
     </row>
     <row r="405" spans="1:23" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A405" s="64" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B405" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C405" s="37" t="s">
         <v>53</v>
@@ -37371,10 +37357,10 @@
     </row>
     <row r="406" spans="1:23" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A406" s="64" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B406" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C406" s="37" t="s">
         <v>53</v>
@@ -37428,10 +37414,10 @@
     </row>
     <row r="407" spans="1:23" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A407" s="64" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B407" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C407" s="37" t="s">
         <v>53</v>
@@ -37485,10 +37471,10 @@
     </row>
     <row r="408" spans="1:23" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A408" s="64" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B408" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C408" s="37" t="s">
         <v>53</v>
@@ -37542,10 +37528,10 @@
     </row>
     <row r="409" spans="1:23" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A409" s="64" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B409" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C409" s="37" t="s">
         <v>53</v>
@@ -37599,10 +37585,10 @@
     </row>
     <row r="410" spans="1:23" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A410" s="64" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B410" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C410" s="37" t="s">
         <v>53</v>
@@ -37656,10 +37642,10 @@
     </row>
     <row r="411" spans="1:23" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A411" s="64" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="B411" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C411" s="37" t="s">
         <v>53</v>
@@ -37713,10 +37699,10 @@
     </row>
     <row r="412" spans="1:23" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A412" s="64" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B412" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C412" s="37" t="s">
         <v>53</v>
@@ -37770,10 +37756,10 @@
     </row>
     <row r="413" spans="1:23" s="24" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A413" s="64" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B413" s="65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C413" s="37" t="s">
         <v>53</v>
@@ -54223,7 +54209,7 @@
     </row>
     <row r="636" spans="1:397" s="30" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A636" s="31" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B636" s="32"/>
       <c r="C636" s="32"/>
@@ -54236,7 +54222,7 @@
       <c r="J636" s="32"/>
       <c r="K636" s="32"/>
       <c r="N636" s="67" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="O636" s="67"/>
       <c r="U636" s="33"/>

</xml_diff>